<commit_message>
feat: initial experiments with max_depth
</commit_message>
<xml_diff>
--- a/documentation/experiment_tracker_xgboost.xlsx
+++ b/documentation/experiment_tracker_xgboost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,44 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>23/06/2022 21:47:29</t>
+          <t>24/06/2022 19:03:38</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Baseline XGBoost</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>XGBoost (v.1)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'max_depth': 9, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.9237,  'validation': 2.6714, 'test': None }, { 'metric': MAE, 'train': 1.3550,  'validation': 1.9234, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>24/06/2022 19:03:39</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Changed max_depth from 10 to 9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: saving best xgb model as pkl file
</commit_message>
<xml_diff>
--- a/documentation/experiment_tracker_xgboost.xlsx
+++ b/documentation/experiment_tracker_xgboost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,17 +478,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'max_depth': 10, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 1, 'gamma': 0, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.300000012, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 1.7643,  'validation': 2.7082, 'test': None }, { 'metric': MAE, 'train': 1.2135,  'validation': 1.9380, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.4729,  'validation': 2.6320, 'test': None }, { 'metric': MAE, 'train': 1.8143,  'validation': 1.9269, 'test': None }]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>24/06/2022 19:03:38</t>
+          <t>01/07/2022 22:14:20</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>XGBoost (v.1)</t>
+          <t>XGBoost 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -510,24 +510,132 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'max_depth': 9, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.200000003, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.2, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 1.9237,  'validation': 2.6714, 'test': None }, { 'metric': MAE, 'train': 1.3550,  'validation': 1.9234, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.4930,  'validation': 2.6233, 'test': None }, { 'metric': MAE, 'train': 1.8292,  'validation': 1.9204, 'test': None }]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>24/06/2022 19:03:39</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Changed max_depth from 10 to 9</t>
-        </is>
-      </c>
+          <t>01/07/2022 22:14:21</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>XGBoost 2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.8872,  'validation': 2.5822, 'test': None }, { 'metric': MAE, 'train': 1.3823,  'validation': 1.8758, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>01/07/2022 22:14:54</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>XGBoost (gamma: 1.5)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.8869,  'validation': 2.5816, 'test': None }, { 'metric': MAE, 'train': 1.3840,  'validation': 1.8753, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>01/07/2022 22:15:29</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>XGBoost (eta: 0.001)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 11, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.6972,  'validation': 2.5873, 'test': None }, { 'metric': MAE, 'train': 1.2327,  'validation': 1.8745, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/07/2022 22:21:59</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>XGBoost (max_depth: 9 and subsample: 0.8)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.8, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.9097,  'validation': 2.5784, 'test': None }, { 'metric': MAE, 'train': 1.3968,  'validation': 1.8723, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>01/07/2022 22:26:55</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: final xgboost models
</commit_message>
<xml_diff>
--- a/documentation/experiment_tracker_xgboost.xlsx
+++ b/documentation/experiment_tracker_xgboost.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 1, 'gamma': 0, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.300000012, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 1, 'gamma': 0, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.300000012, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>02/07/2022 12:11:38</t>
+          <t>04/07/2022 16:04:49</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.200000003, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.2, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.200000003, 'max_delta_step': 0, 'max_depth': 3, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 500, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 1, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.2, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>02/07/2022 12:11:41</t>
+          <t>04/07/2022 16:04:59</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -528,7 +528,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>XGBoost 2</t>
+          <t>XGBoost (max_depth, eta, subsampel and estimators)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>02/07/2022 12:12:31</t>
+          <t>04/07/2022 16:05:51</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>02/07/2022 12:13:22</t>
+          <t>04/07/2022 16:09:05</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -584,7 +584,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>XGBoost (eta: 0.001)</t>
+          <t>XGBoost (max_depth: 7)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -594,17 +594,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 11, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 7, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[{ 'metric': RSME, 'train': 1.6972,  'validation': 2.5873, 'test': None }, { 'metric': MAE, 'train': 1.2327,  'validation': 1.8745, 'test': None }]</t>
+          <t>[{ 'metric': RSME, 'train': 2.1507,  'validation': 2.5762, 'test': None }, { 'metric': MAE, 'train': 1.5812,  'validation': 1.8766, 'test': None }]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>02/07/2022 12:22:43</t>
+          <t>04/07/2022 16:10:02</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -612,30 +612,174 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>XGBoost (- holiday and - peak features)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'timesofday', 'wdsp', 'rainfall_intensity', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 7, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 2.1291,  'validation': 2.5783, 'test': None }, { 'metric': MAE, 'train': 1.5662,  'validation': 1.8773, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:11:20</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>XGBoost (- working_day feat)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'timesofday', 'wdsp', 'rainfall_intensity', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 7, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 2.1735,  'validation': 2.5935, 'test': None }, { 'metric': MAE, 'train': 1.5976,  'validation': 1.8900, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:12:55</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>XGBoost (- season feat)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'timesofday', 'wdsp', 'rainfall_intensity', 'hour', 'working_day']</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00999999978, 'max_delta_step': 0, 'max_depth': 7, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 1000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.01, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 2.2543,  'validation': 2.6297, 'test': None }, { 'metric': MAE, 'train': 1.6586,  'validation': 1.9207, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:13:35</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>XGBoost (eta: 0.001)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 11, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.7, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.6609,  'validation': 2.5881, 'test': None }, { 'metric': MAE, 'train': 1.2083,  'validation': 1.8759, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:21:01</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>XGBoost (max_depth: 9 and subsample: 0.8)</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>['temp', 'rhum', 'dayofweek', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.8, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.8909,  'validation': 2.5797, 'test': None }, { 'metric': MAE, 'train': 1.3838,  'validation': 1.8731, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:25:08</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>XGBoost (only + count values)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>['temp', 'rhum', 'dayofweek', 'holiday', 'timesofday', 'wdsp', 'rainfall_intensity', 'peak', 'working_day', 'hour', 'season']</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 4, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.8, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>[{ 'metric': RSME, 'train': 1.9097,  'validation': 2.5784, 'test': None }, { 'metric': MAE, 'train': 1.3968,  'validation': 1.8723, 'test': None }]</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>02/07/2022 12:30:02</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'objective': 'reg:squarederror', 'base_score': 0.5, 'booster': 'gbtree', 'colsample_bylevel': 1, 'colsample_bynode': 1, 'colsample_bytree': 0.5, 'gamma': 1.5, 'gpu_id': -1, 'importance_type': 'gain', 'interaction_constraints': '', 'learning_rate': 0.00100000005, 'max_delta_step': 0, 'max_depth': 9, 'min_child_weight': 1, 'missing': nan, 'monotone_constraints': '()', 'n_estimators': 5000, 'n_jobs': 12, 'num_parallel_tree': 1, 'random_state': 42, 'reg_alpha': 0, 'reg_lambda': 1, 'scale_pos_weight': 1, 'subsample': 0.8, 'tree_method': 'exact', 'validate_parameters': 1, 'verbosity': None, 'eta': 0.001, 'seed': 42, 'eval_metric': 'rmse'}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>[{ 'metric': RSME, 'train': 1.9839,  'validation': 2.7153, 'test': None }, { 'metric': MAE, 'train': 1.4920,  'validation': 2.0364, 'test': None }]</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>04/07/2022 16:29:20</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Checking possibility of using hurdle model</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: loading pickle pipeline and making predictions on test data
</commit_message>
<xml_diff>
--- a/documentation/experiment_tracker_xgboost.xlsx
+++ b/documentation/experiment_tracker_xgboost.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>04/07/2022 23:00:38</t>
+          <t>05/07/2022 21:16:21</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>04/07/2022 23:00:45</t>
+          <t>05/07/2022 21:16:22</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>04/07/2022 23:01:12</t>
+          <t>05/07/2022 21:16:41</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -576,7 +576,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>04/07/2022 23:01:59</t>
+          <t>05/07/2022 21:17:01</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -604,7 +604,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>04/07/2022 23:03:03</t>
+          <t>05/07/2022 21:17:18</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -632,7 +632,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>04/07/2022 23:03:33</t>
+          <t>05/07/2022 21:17:36</t>
         </is>
       </c>
       <c r="F7" t="inlineStr"/>
@@ -660,7 +660,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>04/07/2022 23:23:55</t>
+          <t>05/07/2022 21:22:01</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>04/07/2022 23:24:17</t>
+          <t>05/07/2022 21:23:22</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -716,7 +716,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>04/07/2022 23:30:24</t>
+          <t>05/07/2022 21:28:09</t>
         </is>
       </c>
       <c r="F10" t="inlineStr"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>04/07/2022 23:35:09</t>
+          <t>05/07/2022 21:31:51</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -772,7 +772,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>04/07/2022 23:38:36</t>
+          <t>05/07/2022 21:35:28</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">

</xml_diff>